<commit_message>
optimalisasi penulisan kode pada pagu 14
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_1.xlsx
+++ b/hasil/2023_01_lipa_1.xlsx
@@ -675,7 +675,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 17 Juli 2023</t>
+    <t>Ternate , 25 Juli 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -4766,7 +4766,7 @@
         <v>49</v>
       </c>
       <c r="D75" s="82" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="E75" s="82" t="s">
         <v>107</v>
@@ -5234,7 +5234,7 @@
         <v>49</v>
       </c>
       <c r="D88" s="82" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="E88" s="82" t="s">
         <v>33</v>
@@ -5488,7 +5488,7 @@
         <v>26</v>
       </c>
       <c r="D95" s="82" t="s">
-        <v>162</v>
+        <v>99</v>
       </c>
       <c r="E95" s="82" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
add func tambah dengan autocomplete pada elitigasi
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_1.xlsx
+++ b/hasil/2023_01_lipa_1.xlsx
@@ -675,7 +675,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 02 Agustus 2023</t>
+    <t>Ternate , 09 Agustus 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -4766,7 +4766,7 @@
         <v>49</v>
       </c>
       <c r="D75" s="82" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="E75" s="82" t="s">
         <v>107</v>
@@ -5234,7 +5234,7 @@
         <v>49</v>
       </c>
       <c r="D88" s="82" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="E88" s="82" t="s">
         <v>33</v>
@@ -5488,7 +5488,7 @@
         <v>26</v>
       </c>
       <c r="D95" s="82" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="E95" s="82" t="s">
         <v>28</v>

</xml_diff>